<commit_message>
A long time spent playing with regex to separate columns
</commit_message>
<xml_diff>
--- a/data/Crossing data summary A_2301 B_1590xQA383P - CLEAN.xlsx
+++ b/data/Crossing data summary A_2301 B_1590xQA383P - CLEAN.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ueahome\eressci1\hpd08ucu\data\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32712D97-F2ED-457A-84AD-C5F45891FD30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEFFA54E-075A-44E7-84C8-D30E616DAD3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1170" windowWidth="28800" windowHeight="14490" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="225" windowWidth="28800" windowHeight="14490" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="F1" sheetId="1" r:id="rId1"/>
@@ -28595,11 +28595,11 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="D3:L3"/>
-    <mergeCell ref="O3:R3"/>
-    <mergeCell ref="S3:V3"/>
-    <mergeCell ref="D33:G33"/>
-    <mergeCell ref="D34:G34"/>
+    <mergeCell ref="D47:G47"/>
+    <mergeCell ref="D48:G48"/>
+    <mergeCell ref="D49:G49"/>
+    <mergeCell ref="D50:G50"/>
+    <mergeCell ref="D51:G51"/>
     <mergeCell ref="D35:G35"/>
     <mergeCell ref="D36:G36"/>
     <mergeCell ref="D44:G44"/>
@@ -28612,11 +28612,11 @@
     <mergeCell ref="D41:G41"/>
     <mergeCell ref="D42:G42"/>
     <mergeCell ref="D43:G43"/>
-    <mergeCell ref="D47:G47"/>
-    <mergeCell ref="D48:G48"/>
-    <mergeCell ref="D49:G49"/>
-    <mergeCell ref="D50:G50"/>
-    <mergeCell ref="D51:G51"/>
+    <mergeCell ref="D3:L3"/>
+    <mergeCell ref="O3:R3"/>
+    <mergeCell ref="S3:V3"/>
+    <mergeCell ref="D33:G33"/>
+    <mergeCell ref="D34:G34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -28628,7 +28628,7 @@
   <dimension ref="A1:AC1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:C54"/>
+      <selection activeCell="C4" sqref="C4:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -28706,9 +28706,6 @@
     <row r="3" spans="1:29" ht="14.25" customHeight="1">
       <c r="A3" s="1"/>
       <c r="B3" s="10"/>
-      <c r="C3" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
         <v>26</v>
@@ -28752,8 +28749,8 @@
       <c r="A4" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="11" t="s">
-        <v>23</v>
+      <c r="C4" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>19</v>
@@ -28831,6 +28828,9 @@
     <row r="5" spans="1:29" ht="14.25" customHeight="1">
       <c r="A5" s="11" t="s">
         <v>25</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>23</v>
       </c>
       <c r="D5" s="11">
         <v>1</v>
@@ -61103,11 +61103,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="F3:O3"/>
-    <mergeCell ref="R3:U3"/>
-    <mergeCell ref="W3:Z3"/>
-    <mergeCell ref="R129:U129"/>
-    <mergeCell ref="W129:Z129"/>
     <mergeCell ref="F179:O179"/>
     <mergeCell ref="R179:U179"/>
     <mergeCell ref="W179:Z179"/>
@@ -61118,6 +61113,11 @@
     <mergeCell ref="R103:U103"/>
     <mergeCell ref="W103:Z103"/>
     <mergeCell ref="F129:O129"/>
+    <mergeCell ref="F3:O3"/>
+    <mergeCell ref="R3:U3"/>
+    <mergeCell ref="W3:Z3"/>
+    <mergeCell ref="R129:U129"/>
+    <mergeCell ref="W129:Z129"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>